<commit_message>
Add more information to this file
</commit_message>
<xml_diff>
--- a/tennis_match_chart_symbols_col_description.xlsx
+++ b/tennis_match_chart_symbols_col_description.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/NO NAME/Programming/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yingz\Python_files\tenantics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B84090-E499-454C-9A81-E212DC11FA1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230CEDCE-0B22-47D3-BB78-C176D6777A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="5940" windowWidth="26860" windowHeight="12360" activeTab="1" xr2:uid="{7182A60C-9168-42F6-9FFE-C16DF5B2BAC1}"/>
+    <workbookView xWindow="6405" yWindow="315" windowWidth="27285" windowHeight="13545" activeTab="1" xr2:uid="{7182A60C-9168-42F6-9FFE-C16DF5B2BAC1}"/>
   </bookViews>
   <sheets>
     <sheet name="symbol description" sheetId="1" r:id="rId1"/>
     <sheet name="colmn description" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" calcCompleted="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -490,9 +490,6 @@
     <t>Game index for the current match, reset after each match (point index for the current game, reset after each game)</t>
   </si>
   <si>
-    <t>1 means the current point is played in a tiebreak, otherwise 0. This helps you interpret the score in the "Pts" column.</t>
-  </si>
-  <si>
     <t>Point index within the current tiebreak, reset after the tiebreak</t>
   </si>
   <si>
@@ -624,9 +621,6 @@
 MatchChart 0.3.2.xlsm explains the coding used in the Excel sheet. </t>
   </si>
   <si>
-    <t>Almost always 1, whether the final set has a tiebreak at the end or not (only French Open does not have tiebreak at end of final set)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coded sequence of shots from the first serve, including the serve. Use the symbol description in the other worksheet to interpret the codes. This is the main entry. Almost everything else is derived from here. </t>
   </si>
   <si>
@@ -643,6 +637,12 @@
   </si>
   <si>
     <t>Score after the point is finished. In tiebreak, when server switches, the score also switches to display the server's score first. If the game is done, "GM" will appear here.</t>
+  </si>
+  <si>
+    <t>Almost always 1, whether the final set has a tiebreak at the end or not (only French Open does not have tiebreak at end of final set). 1 means the final set is decided by a tiebreak. 0 means the final set is not decided by a tiebreak. S means the final set is decided by a 10 point super-tiebreak. W means the tiebreak is played at 8-8. V means no tie-break is played in any set.</t>
+  </si>
+  <si>
+    <t>1 means the current point is played in a tiebreak, otherwise 0. This helps you interpret the score in the "Pts" column. S means this is a 10-point super-tiebreak.</t>
   </si>
 </sst>
 </file>
@@ -1032,20 +1032,20 @@
       <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="95" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>8</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>9</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>93</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>95</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>98</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>99</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>102</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>104</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>106</v>
       </c>
@@ -1546,35 +1546,35 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>191</v>
+      </c>
+      <c r="B64" t="s">
         <v>192</v>
       </c>
-      <c r="B64" t="s">
+    </row>
+    <row r="65" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="208" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="B65" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B70" s="3"/>
     </row>
   </sheetData>
@@ -1589,12 +1589,12 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ2" sqref="AJ2"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -1745,120 +1745,120 @@
         <v>152</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>153</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="X2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="V2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="X2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="AJ2" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>183</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1876,10 +1876,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" t="s">
         <v>184</v>
-      </c>
-      <c r="H3" t="s">
-        <v>185</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1894,13 +1894,13 @@
         <v>2</v>
       </c>
       <c r="N3" t="s">
+        <v>185</v>
+      </c>
+      <c r="O3" t="s">
         <v>186</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>187</v>
-      </c>
-      <c r="P3" t="s">
-        <v>188</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -1921,13 +1921,13 @@
         <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Y3">
         <v>6</v>
       </c>
       <c r="Z3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AA3" t="b">
         <v>0</v>
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="AJ3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AK3">
         <v>0</v>

</xml_diff>